<commit_message>
add feature list and FE2
</commit_message>
<xml_diff>
--- a/code/featureList.xlsx
+++ b/code/featureList.xlsx
@@ -181,12 +181,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,9 +195,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,84 +218,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -301,19 +240,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -325,22 +315,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,13 +348,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,169 +528,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,6 +539,24 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -564,17 +575,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,216 +625,175 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1161,8 +1151,8 @@
   <sheetPr/>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -1278,7 +1268,7 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
@@ -1289,7 +1279,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="3"/>
+      <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -1298,7 +1288,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="3"/>
+      <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -1307,19 +1297,19 @@
       </c>
     </row>
     <row r="18" ht="108" spans="1:4">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B19" t="s">
@@ -1330,19 +1320,19 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="3"/>
+      <c r="A20" s="1"/>
       <c r="B20" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="3"/>
+      <c r="A21" s="1"/>
       <c r="B21" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="3"/>
+      <c r="A22" s="1"/>
       <c r="B22" t="s">
         <v>30</v>
       </c>
@@ -1351,19 +1341,19 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="3"/>
+      <c r="A23" s="1"/>
       <c r="B23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="3"/>
+      <c r="A24" s="1"/>
       <c r="B24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="3"/>
+      <c r="A25" s="1"/>
       <c r="B25" t="s">
         <v>33</v>
       </c>
@@ -1372,19 +1362,19 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="3"/>
+      <c r="A26" s="1"/>
       <c r="B26" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="3"/>
+      <c r="A27" s="1"/>
       <c r="B27" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="3"/>
+      <c r="A28" s="1"/>
       <c r="B28" t="s">
         <v>36</v>
       </c>
@@ -1393,19 +1383,19 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="3"/>
+      <c r="A29" s="1"/>
       <c r="B29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="3"/>
+      <c r="A30" s="1"/>
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="3"/>
+      <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>39</v>
       </c>
@@ -1414,19 +1404,19 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="3"/>
+      <c r="A32" s="1"/>
       <c r="B32" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="3"/>
+      <c r="A33" s="1"/>
       <c r="B33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="3"/>
+      <c r="A34" s="1"/>
       <c r="B34" t="s">
         <v>42</v>
       </c>
@@ -1435,19 +1425,19 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="3"/>
+      <c r="A35" s="1"/>
       <c r="B35" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="3"/>
+      <c r="A36" s="1"/>
       <c r="B36" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="3"/>
+      <c r="A37" s="1"/>
       <c r="B37" t="s">
         <v>45</v>
       </c>
@@ -1456,19 +1446,19 @@
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="3"/>
+      <c r="A38" s="1"/>
       <c r="B38" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="3"/>
+      <c r="A39" s="1"/>
       <c r="B39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="3"/>
+      <c r="A40" s="1"/>
       <c r="B40" t="s">
         <v>48</v>
       </c>
@@ -1477,13 +1467,13 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="3"/>
+      <c r="A41" s="1"/>
       <c r="B41" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="3"/>
+      <c r="A42" s="1"/>
       <c r="B42" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
add first online result
</commit_message>
<xml_diff>
--- a/code/featureList.xlsx
+++ b/code/featureList.xlsx
@@ -179,8 +179,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -192,48 +192,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -242,72 +200,100 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -321,22 +307,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,187 +351,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,11 +566,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -586,6 +631,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -594,64 +648,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -660,137 +666,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -799,10 +805,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1155,8 +1162,8 @@
   <sheetPr/>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -1275,44 +1282,47 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1"/>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1"/>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" ht="108" spans="1:4">
       <c r="A18" s="1"/>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>